<commit_message>
Update and added new point to better align railway
</commit_message>
<xml_diff>
--- a/hwy_data/NLD/nldrail/export.xlsx
+++ b/hwy_data/NLD/nldrail/export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bart.roem\Github\HighwayData\hwy_data\NLD\nldrail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3156C669-C91C-49AA-AFC5-91E4438F6C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC42C96-00AD-4479-9851-B76B0CC30D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10600" yWindow="3670" windowWidth="28800" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="export" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3200" uniqueCount="1592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216" uniqueCount="1611">
   <si>
     <t>Afk.</t>
   </si>
@@ -4776,9 +4776,6 @@
     <t>Gevonden naam</t>
   </si>
   <si>
-    <t>weesp</t>
-  </si>
-  <si>
     <t>almere p</t>
   </si>
   <si>
@@ -4807,6 +4804,66 @@
   </si>
   <si>
     <t>zwoll</t>
+  </si>
+  <si>
+    <t>Openstreetmap input</t>
+  </si>
+  <si>
+    <t>output link</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/52.7277803/4.8438043</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/53.2125986/6.4872402</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/52.3929810/4.6223406</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/52.4557170/4.6564645</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/52.5147816/4.7085732</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/53.1892577/5.7491641</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/51.4417919/6.1279482</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/53.4625909/6.8153347</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/51.4405738/4.2949909</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/52.5491430/5.4956482</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/52.6221263/6.2407127</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/53.0675927/6.6280127</t>
+  </si>
+  <si>
+    <t>ah</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>herto</t>
+  </si>
+  <si>
+    <t>ht</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/52.1948371/6.2371089</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/#map=18/51.8594427/5.2627501</t>
   </si>
 </sst>
 </file>
@@ -5290,9 +5347,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5338,7 +5396,15 @@
     <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -5384,7 +5450,7 @@
   <autoFilter ref="O1:P35" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Afkorting"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Lijst voor travelmapping" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Lijst voor travelmapping" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.IFNA(VLOOKUP(Tabel2[[#This Row],[Afkorting]],Tabel1[],9,FALSE),Tabel2[[#This Row],[Afkorting]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5408,11 +5474,24 @@
   <autoFilter ref="K1:M14" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Stationsnaam"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Afkorting" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Afkorting" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Gevonden naam" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Gevonden naam" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP(Tabel4[[#This Row],[Afkorting]],Tabel1[],8,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5B83DD41-DD57-4C85-B5FC-F7909ED6E354}" name="Tabel5" displayName="Tabel5" ref="U1:V47" totalsRowShown="0">
+  <autoFilter ref="U1:V47" xr:uid="{5B83DD41-DD57-4C85-B5FC-F7909ED6E354}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6372F51E-B143-4EA4-A592-53614282291C}" name="Openstreetmap input" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{0525D0D6-F8EF-4F77-BCDE-965BD06E0365}" name="output link">
+      <calculatedColumnFormula>"https://www.openstreetmap.org/" &amp; "?lat=" &amp; LEFT(RIGHT(U2,20),10) &amp; "&amp;lon=" &amp; RIGHT(U2,9)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5716,10 +5795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S548"/>
+  <dimension ref="A1:V548"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5737,9 +5816,11 @@
     <col min="16" max="16" width="62.7265625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.36328125" customWidth="1"/>
     <col min="19" max="19" width="10.6328125" customWidth="1"/>
+    <col min="21" max="21" width="57.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5788,8 +5869,14 @@
       <c r="S1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U1" t="s">
+        <v>1591</v>
+      </c>
+      <c r="V1" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -5814,23 +5901,23 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
-        <v>1581</v>
-      </c>
-      <c r="L2" t="str">
+      <c r="K2" s="1" t="s">
+        <v>1607</v>
+      </c>
+      <c r="L2" t="e">
         <f>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</f>
-        <v>Wp</v>
-      </c>
-      <c r="M2" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M2" t="e">
         <f>VLOOKUP(Tabel4[[#This Row],[Afkorting]],Tabel1[],8,FALSE)</f>
-        <v>Weesp</v>
+        <v>#N/A</v>
       </c>
       <c r="O2" t="s">
-        <v>1357</v>
+        <v>1606</v>
       </c>
       <c r="P2" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Tabel2[[#This Row],[Afkorting]],Tabel1[],9,FALSE),Tabel2[[#This Row],[Afkorting]])</f>
-        <v>Wp https://www.openstreetmap.org/?lat=52.3122067&amp;lon=5.0440484</v>
+        <v>Nm https://www.openstreetmap.org/?lat=51.8431362&amp;lon=5.8530913</v>
       </c>
       <c r="R2" t="s">
         <v>11</v>
@@ -5838,8 +5925,15 @@
       <c r="S2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U2" s="2" t="s">
+        <v>1593</v>
+      </c>
+      <c r="V2" t="str">
+        <f>"https://www.openstreetmap.org/" &amp; "?lat=" &amp; LEFT(RIGHT(U2,20),10) &amp; "&amp;lon=" &amp; RIGHT(U2,9)</f>
+        <v>https://www.openstreetmap.org/?lat=52.7277803&amp;lon=4.8438043</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -5865,7 +5959,7 @@
         <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="L3" t="str">
         <f>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</f>
@@ -5876,11 +5970,11 @@
         <v>Almere Poort</v>
       </c>
       <c r="O3" t="s">
-        <v>289</v>
+        <v>1608</v>
       </c>
       <c r="P3" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Tabel2[[#This Row],[Afkorting]],Tabel1[],9,FALSE),Tabel2[[#This Row],[Afkorting]])</f>
-        <v>Ampo https://www.openstreetmap.org/?lat=52.3429466&amp;lon=5.1522517</v>
+        <v>Ht https://www.openstreetmap.org/?lat=51.6905164&amp;lon=5.2937086</v>
       </c>
       <c r="R3" t="s">
         <v>16</v>
@@ -5888,8 +5982,15 @@
       <c r="S3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U3" s="2" t="s">
+        <v>1594</v>
+      </c>
+      <c r="V3" t="str">
+        <f t="shared" ref="V3:V47" si="0">"https://www.openstreetmap.org/" &amp; "?lat=" &amp; LEFT(RIGHT(U3,20),10) &amp; "&amp;lon=" &amp; RIGHT(U3,9)</f>
+        <v>https://www.openstreetmap.org/?lat=53.2125986&amp;lon=6.4872402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -5915,7 +6016,7 @@
         <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="L4" t="str">
         <f>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</f>
@@ -5926,11 +6027,11 @@
         <v>Almere Muziekwijk</v>
       </c>
       <c r="O4" t="s">
-        <v>1354</v>
+        <v>1605</v>
       </c>
       <c r="P4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Tabel2[[#This Row],[Afkorting]],Tabel1[],9,FALSE),Tabel2[[#This Row],[Afkorting]])</f>
-        <v>Almm https://www.openstreetmap.org/?lat=52.367558&amp;lon=5.190341</v>
+        <v>Ah https://www.openstreetmap.org/?lat=51.9844332&amp;lon=5.9011598</v>
       </c>
       <c r="R4" t="s">
         <v>20</v>
@@ -5938,8 +6039,15 @@
       <c r="S4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U4" s="2" t="s">
+        <v>1595</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=52.3929810&amp;lon=4.6223406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -5965,7 +6073,7 @@
         <v>25</v>
       </c>
       <c r="K5" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="L5" t="str">
         <f>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</f>
@@ -5988,8 +6096,15 @@
       <c r="S5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U5" s="2" t="s">
+        <v>1596</v>
+      </c>
+      <c r="V5" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=52.4557170&amp;lon=4.6564645</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -6015,7 +6130,7 @@
         <v>29</v>
       </c>
       <c r="K6" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="L6" t="str">
         <f>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</f>
@@ -6038,8 +6153,15 @@
       <c r="S6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U6" s="2" t="s">
+        <v>1597</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=52.5147816&amp;lon=4.7085732</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -6065,7 +6187,7 @@
         <v>33</v>
       </c>
       <c r="K7" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="L7" t="str">
         <f>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</f>
@@ -6088,8 +6210,15 @@
       <c r="S7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U7" s="2" t="s">
+        <v>1598</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=53.1892577&amp;lon=5.7491641</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -6115,7 +6244,7 @@
         <v>34</v>
       </c>
       <c r="K8" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="L8" t="str">
         <f>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</f>
@@ -6138,8 +6267,15 @@
       <c r="S8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U8" s="2" t="s">
+        <v>1599</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=51.4417919&amp;lon=6.1279482</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -6165,7 +6301,7 @@
         <v>40</v>
       </c>
       <c r="K9" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="L9" t="str">
         <f>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</f>
@@ -6188,8 +6324,15 @@
       <c r="S9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U9" s="2" t="s">
+        <v>1600</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=53.4625909&amp;lon=6.8153347</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -6215,7 +6358,7 @@
         <v>30</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="L10" t="str">
         <f>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</f>
@@ -6238,8 +6381,15 @@
       <c r="S10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U10" s="2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=51.4405738&amp;lon=4.2949909</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -6265,7 +6415,7 @@
         <v>47</v>
       </c>
       <c r="K11" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="L11" t="str">
         <f>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</f>
@@ -6288,8 +6438,15 @@
       <c r="S11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U11" s="2" t="s">
+        <v>1602</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=52.5491430&amp;lon=5.4956482</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -6315,7 +6472,7 @@
         <v>14</v>
       </c>
       <c r="K12" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="L12" t="str">
         <f>VLOOKUP(Tabel4[[#This Row],[Stationsnaam]]&amp;"*",Tabel3[],2,FALSE)</f>
@@ -6338,8 +6495,15 @@
       <c r="S12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U12" s="2" t="s">
+        <v>1603</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=52.6221263&amp;lon=6.2407127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -6382,8 +6546,15 @@
       <c r="S13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U13" s="2" t="s">
+        <v>1604</v>
+      </c>
+      <c r="V13" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=53.0675927&amp;lon=6.6280127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -6426,8 +6597,15 @@
       <c r="S14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U14" s="2" t="s">
+        <v>1609</v>
+      </c>
+      <c r="V14" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=52.1948371&amp;lon=6.2371089</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -6462,8 +6640,15 @@
       <c r="S15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U15" s="2" t="s">
+        <v>1610</v>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=51.8594427&amp;lon=5.2627501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -6498,8 +6683,13 @@
       <c r="S16" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U16" s="2"/>
+      <c r="V16" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -6534,8 +6724,13 @@
       <c r="S17" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U17" s="2"/>
+      <c r="V17" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -6570,8 +6765,13 @@
       <c r="S18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U18" s="2"/>
+      <c r="V18" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -6606,8 +6806,13 @@
       <c r="S19" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U19" s="2"/>
+      <c r="V19" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -6642,8 +6847,13 @@
       <c r="S20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U20" s="2"/>
+      <c r="V20" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -6678,8 +6888,13 @@
       <c r="S21" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U21" s="2"/>
+      <c r="V21" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -6714,8 +6929,13 @@
       <c r="S22" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U22" s="2"/>
+      <c r="V22" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -6750,8 +6970,13 @@
       <c r="S23" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U23" s="2"/>
+      <c r="V23" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -6786,8 +7011,13 @@
       <c r="S24" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U24" s="2"/>
+      <c r="V24" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -6822,8 +7052,13 @@
       <c r="S25" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U25" s="2"/>
+      <c r="V25" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -6858,8 +7093,13 @@
       <c r="S26" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U26" s="2"/>
+      <c r="V26" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>96</v>
       </c>
@@ -6894,8 +7134,13 @@
       <c r="S27" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U27" s="2"/>
+      <c r="V27" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -6930,8 +7175,13 @@
       <c r="S28" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U28" s="2"/>
+      <c r="V28" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -6966,8 +7216,13 @@
       <c r="S29" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U29" s="2"/>
+      <c r="V29" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>105</v>
       </c>
@@ -7002,8 +7257,13 @@
       <c r="S30" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U30" s="2"/>
+      <c r="V30" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>108</v>
       </c>
@@ -7038,8 +7298,13 @@
       <c r="S31" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U31" s="2"/>
+      <c r="V31" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -7074,8 +7339,13 @@
       <c r="S32" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U32" s="2"/>
+      <c r="V32" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -7110,8 +7380,13 @@
       <c r="S33" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U33" s="2"/>
+      <c r="V33" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -7146,8 +7421,13 @@
       <c r="S34" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U34" s="2"/>
+      <c r="V34" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>120</v>
       </c>
@@ -7182,8 +7462,13 @@
       <c r="S35" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U35" s="2"/>
+      <c r="V35" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>123</v>
       </c>
@@ -7214,8 +7499,13 @@
       <c r="S36" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U36" s="2"/>
+      <c r="V36" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>126</v>
       </c>
@@ -7246,8 +7536,13 @@
       <c r="S37" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U37" s="2"/>
+      <c r="V37" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>129</v>
       </c>
@@ -7278,8 +7573,13 @@
       <c r="S38" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U38" s="2"/>
+      <c r="V38" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -7310,8 +7610,13 @@
       <c r="S39" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U39" s="2"/>
+      <c r="V39" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>135</v>
       </c>
@@ -7342,8 +7647,13 @@
       <c r="S40" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U40" s="2"/>
+      <c r="V40" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>138</v>
       </c>
@@ -7374,8 +7684,13 @@
       <c r="S41" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U41" s="2"/>
+      <c r="V41" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>141</v>
       </c>
@@ -7406,8 +7721,13 @@
       <c r="S42" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U42" s="2"/>
+      <c r="V42" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>144</v>
       </c>
@@ -7438,8 +7758,13 @@
       <c r="S43" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U43" s="2"/>
+      <c r="V43" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>147</v>
       </c>
@@ -7470,8 +7795,13 @@
       <c r="S44" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U44" s="2"/>
+      <c r="V44" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>150</v>
       </c>
@@ -7502,8 +7832,13 @@
       <c r="S45" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U45" s="2"/>
+      <c r="V45" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>153</v>
       </c>
@@ -7534,8 +7869,13 @@
       <c r="S46" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U46" s="2"/>
+      <c r="V46" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>156</v>
       </c>
@@ -7566,8 +7906,13 @@
       <c r="S47" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U47" s="2"/>
+      <c r="V47" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.openstreetmap.org/?lat=&amp;lon=</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>159</v>
       </c>
@@ -23301,11 +23646,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>